<commit_message>
Fix a few bugs, clean up a few things
</commit_message>
<xml_diff>
--- a/adab data.xlsx
+++ b/adab data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\ADAnswers-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFFE751-E974-4C3E-A75B-77C61E2B61AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221B7DDC-93F9-467B-953E-1410230CDA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{2F0C51A9-9C83-4846-B7AE-2F85BD881AF9}"/>
   </bookViews>
@@ -17,17 +17,19 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$15:$B$38</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$15:$C$38</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$15:$C$38</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$O$37</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$15:$C$38</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Table1!$A$1:$B$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -59,7 +61,7 @@
     <t>Since the beginning of data collection, the bot has been used</t>
   </si>
   <si>
-    <t>Last updated at 16:35 on Friday, September 14, 2021</t>
+    <t>Last updated at 09:15 on Saturday, October 2, 2021</t>
   </si>
 </sst>
 </file>
@@ -170,10 +172,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="107"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="7"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -202,7 +204,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> an ADAnswersBot command has been used based on hour in UTC-5 (as of 16:35 on Friday, September 14, 2021)</a:t>
+              <a:t> an ADAnswersBot command has been used based on hour in UTC-5 (as of 09:15 on Saturday, October 2, 2021)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -249,7 +251,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent5"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -345,76 +347,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>142</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>155</c:v>
+                  <c:v>189</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>157</c:v>
+                  <c:v>229</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>182</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>149</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>166</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>237</c:v>
+                  <c:v>278</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>246</c:v>
+                  <c:v>325</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>204</c:v>
+                  <c:v>304</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>248</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>263</c:v>
+                  <c:v>335</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>366</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>359</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>288</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>244</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>239</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>301</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>240</c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>230</c:v>
+                  <c:v>273</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>234</c:v>
+                  <c:v>279</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>237</c:v>
+                  <c:v>291</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>250</c:v>
+                  <c:v>305</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>229</c:v>
+                  <c:v>288</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>181</c:v>
+                  <c:v>251</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>240</c:v>
+                  <c:v>279</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>215</c:v>
+                  <c:v>238</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -750,7 +752,13 @@
               <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Times an ADAnswersBot command has been used based on hour in UTC-5 (as of 16:35 on Friday, September 14, 2021)</a:t>
+              <a:t>Times an ADAnswersBot command has been used based on hour in UTC-5 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(as of 09:15 on Saturday, October 2, 2021)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
               <a:effectLst/>
@@ -1467,76 +1475,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>142</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>155</c:v>
+                  <c:v>189</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>157</c:v>
+                  <c:v>229</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>182</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>149</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>166</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>237</c:v>
+                  <c:v>278</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>246</c:v>
+                  <c:v>325</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>204</c:v>
+                  <c:v>304</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>248</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>263</c:v>
+                  <c:v>335</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>366</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>359</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>288</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>244</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>239</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>301</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>240</c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>230</c:v>
+                  <c:v>273</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>234</c:v>
+                  <c:v>279</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>237</c:v>
+                  <c:v>291</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>250</c:v>
+                  <c:v>305</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>229</c:v>
+                  <c:v>288</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>181</c:v>
+                  <c:v>251</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>240</c:v>
+                  <c:v>279</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>215</c:v>
+                  <c:v>238</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1612,42 +1620,8 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="25">
   <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -3352,7 +3326,7 @@
   <dimension ref="B4:AB39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3388,7 +3362,7 @@
       </c>
       <c r="E6" s="2">
         <f>SUM(C15, C16, C17, C18, C19, C20, C21, C22, C23, C24, C25, C26, C27, C28, C29, C30, C31, C32, C33, C34, C35, C36, C37, C38)</f>
-        <v>5277</v>
+        <v>6667</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>2</v>
@@ -3463,7 +3437,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>142</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.25">
@@ -3471,7 +3445,7 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>155</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -3479,7 +3453,7 @@
         <v>2</v>
       </c>
       <c r="C17">
-        <v>157</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -3487,7 +3461,7 @@
         <v>3</v>
       </c>
       <c r="C18">
-        <v>182</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -3495,7 +3469,7 @@
         <v>4</v>
       </c>
       <c r="C19">
-        <v>149</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -3503,7 +3477,7 @@
         <v>5</v>
       </c>
       <c r="C20">
-        <v>166</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -3511,7 +3485,7 @@
         <v>6</v>
       </c>
       <c r="C21">
-        <v>237</v>
+        <v>278</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
@@ -3519,7 +3493,7 @@
         <v>7</v>
       </c>
       <c r="C22">
-        <v>246</v>
+        <v>325</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
@@ -3527,7 +3501,7 @@
         <v>8</v>
       </c>
       <c r="C23">
-        <v>204</v>
+        <v>304</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
@@ -3535,7 +3509,7 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <v>248</v>
+        <v>300</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
@@ -3543,7 +3517,7 @@
         <v>10</v>
       </c>
       <c r="C25">
-        <v>263</v>
+        <v>335</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
@@ -3551,7 +3525,7 @@
         <v>11</v>
       </c>
       <c r="C26">
-        <v>288</v>
+        <v>366</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
@@ -3559,7 +3533,7 @@
         <v>12</v>
       </c>
       <c r="C27">
-        <v>244</v>
+        <v>305</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
@@ -3567,7 +3541,7 @@
         <v>13</v>
       </c>
       <c r="C28">
-        <v>239</v>
+        <v>359</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -3575,7 +3549,7 @@
         <v>14</v>
       </c>
       <c r="C29">
-        <v>301</v>
+        <v>352</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
@@ -3583,7 +3557,7 @@
         <v>15</v>
       </c>
       <c r="C30">
-        <v>240</v>
+        <v>288</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
@@ -3591,7 +3565,7 @@
         <v>16</v>
       </c>
       <c r="C31">
-        <v>230</v>
+        <v>273</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
@@ -3599,7 +3573,7 @@
         <v>17</v>
       </c>
       <c r="C32">
-        <v>234</v>
+        <v>279</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
@@ -3607,7 +3581,7 @@
         <v>18</v>
       </c>
       <c r="C33">
-        <v>237</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
@@ -3615,7 +3589,7 @@
         <v>19</v>
       </c>
       <c r="C34">
-        <v>250</v>
+        <v>305</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
@@ -3623,7 +3597,7 @@
         <v>20</v>
       </c>
       <c r="C35">
-        <v>229</v>
+        <v>288</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
@@ -3631,7 +3605,7 @@
         <v>21</v>
       </c>
       <c r="C36">
-        <v>181</v>
+        <v>251</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
@@ -3639,7 +3613,7 @@
         <v>22</v>
       </c>
       <c r="C37">
-        <v>240</v>
+        <v>279</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
@@ -3647,13 +3621,13 @@
         <v>23</v>
       </c>
       <c r="C38">
-        <v>215</v>
+        <v>238</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E39">
         <f>SUM(C15, C16, C17, C18, C19, C20, C21, C22, C23, C24, C25, C26, C27, C28, C29, C30, C31, C32, C33, C34, C35, C36, C37, C38)</f>
-        <v>5277</v>
+        <v>6667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix a bunch of trailing spaces problems, move code around
</commit_message>
<xml_diff>
--- a/adab data.xlsx
+++ b/adab data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\ADAnswers-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A0CCEB-F54D-470C-82DD-A889D355CE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAABD638-04AB-445A-98CB-8F4BB8628E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{2F0C51A9-9C83-4846-B7AE-2F85BD881AF9}"/>
   </bookViews>
@@ -61,7 +61,7 @@
     <t>Since the beginning of data collection, the bot has been used</t>
   </si>
   <si>
-    <t>Last updated at 22:30 on Saturday, October 9, 2021</t>
+    <t>Last updated at 08:36 on Monday, October 25, 2021</t>
   </si>
 </sst>
 </file>
@@ -204,7 +204,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> an ADAnswersBot command has been used based on hour in UTC-5 (as of 22:30 on Saturday, October 9, 2021)</a:t>
+              <a:t> an ADAnswersBot command has been used based on hour in UTC-5 (as of 08:36 on Monday, October 25, 2021)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -347,76 +347,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>217</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>233</c:v>
+                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>273</c:v>
+                  <c:v>319</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>264</c:v>
+                  <c:v>337</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>251</c:v>
+                  <c:v>352</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>273</c:v>
+                  <c:v>408</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>317</c:v>
+                  <c:v>454</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>372</c:v>
+                  <c:v>524</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>366</c:v>
+                  <c:v>521</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>365</c:v>
+                  <c:v>476</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>429</c:v>
+                  <c:v>569</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>418</c:v>
+                  <c:v>570</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>359</c:v>
+                  <c:v>475</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>321</c:v>
+                  <c:v>455</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>539</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>528</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>528</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>517</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>453</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>483</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>459</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>420</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>364</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>334</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>374</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>391</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>350</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>349</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>350</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>333</c:v>
-                </c:pt>
                 <c:pt idx="23">
-                  <c:v>274</c:v>
+                  <c:v>380</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -758,7 +758,7 @@
               <a:rPr lang="en-US" sz="1800" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>(as of 22:30 on Saturday, October 9, 2021)</a:t>
+              <a:t>(as of 08:36 on Monday, October 25, 2021)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
               <a:effectLst/>
@@ -1475,76 +1475,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>217</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>233</c:v>
+                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>273</c:v>
+                  <c:v>319</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>264</c:v>
+                  <c:v>337</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>251</c:v>
+                  <c:v>352</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>273</c:v>
+                  <c:v>408</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>317</c:v>
+                  <c:v>454</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>372</c:v>
+                  <c:v>524</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>366</c:v>
+                  <c:v>521</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>365</c:v>
+                  <c:v>476</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>429</c:v>
+                  <c:v>569</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>418</c:v>
+                  <c:v>570</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>359</c:v>
+                  <c:v>475</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>321</c:v>
+                  <c:v>455</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>539</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>528</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>528</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>517</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>453</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>483</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>459</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>420</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>364</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>334</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>374</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>391</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>350</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>349</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>350</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>333</c:v>
-                </c:pt>
                 <c:pt idx="23">
-                  <c:v>274</c:v>
+                  <c:v>380</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3326,7 +3326,7 @@
   <dimension ref="B4:AB39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+      <selection activeCell="AG26" sqref="AG26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3362,7 +3362,7 @@
       </c>
       <c r="E6" s="2">
         <f>SUM(C15, C16, C17, C18, C19, C20, C21, C22, C23, C24, C25, C26, C27, C28, C29, C30, C31, C32, C33, C34, C35, C36, C37, C38)</f>
-        <v>7997</v>
+        <v>10805</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>2</v>
@@ -3437,7 +3437,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>217</v>
+        <v>286</v>
       </c>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.25">
@@ -3445,7 +3445,7 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>233</v>
+        <v>302</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -3453,7 +3453,7 @@
         <v>2</v>
       </c>
       <c r="C17">
-        <v>273</v>
+        <v>319</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -3461,7 +3461,7 @@
         <v>3</v>
       </c>
       <c r="C18">
-        <v>264</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -3469,7 +3469,7 @@
         <v>4</v>
       </c>
       <c r="C19">
-        <v>251</v>
+        <v>352</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -3477,7 +3477,7 @@
         <v>5</v>
       </c>
       <c r="C20">
-        <v>273</v>
+        <v>408</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -3485,7 +3485,7 @@
         <v>6</v>
       </c>
       <c r="C21">
-        <v>317</v>
+        <v>454</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
@@ -3493,7 +3493,7 @@
         <v>7</v>
       </c>
       <c r="C22">
-        <v>372</v>
+        <v>524</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
@@ -3501,7 +3501,7 @@
         <v>8</v>
       </c>
       <c r="C23">
-        <v>366</v>
+        <v>521</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
@@ -3509,7 +3509,7 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <v>365</v>
+        <v>476</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
@@ -3517,7 +3517,7 @@
         <v>10</v>
       </c>
       <c r="C25">
-        <v>429</v>
+        <v>569</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
@@ -3525,7 +3525,7 @@
         <v>11</v>
       </c>
       <c r="C26">
-        <v>418</v>
+        <v>570</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
@@ -3533,7 +3533,7 @@
         <v>12</v>
       </c>
       <c r="C27">
-        <v>359</v>
+        <v>475</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
@@ -3541,7 +3541,7 @@
         <v>13</v>
       </c>
       <c r="C28">
-        <v>321</v>
+        <v>455</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -3549,7 +3549,7 @@
         <v>14</v>
       </c>
       <c r="C29">
-        <v>420</v>
+        <v>539</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
@@ -3557,7 +3557,7 @@
         <v>15</v>
       </c>
       <c r="C30">
-        <v>364</v>
+        <v>528</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
@@ -3565,7 +3565,7 @@
         <v>16</v>
       </c>
       <c r="C31">
-        <v>334</v>
+        <v>450</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
@@ -3573,7 +3573,7 @@
         <v>17</v>
       </c>
       <c r="C32">
-        <v>374</v>
+        <v>528</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
@@ -3581,7 +3581,7 @@
         <v>18</v>
       </c>
       <c r="C33">
-        <v>391</v>
+        <v>517</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
@@ -3589,7 +3589,7 @@
         <v>19</v>
       </c>
       <c r="C34">
-        <v>350</v>
+        <v>453</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
@@ -3597,7 +3597,7 @@
         <v>20</v>
       </c>
       <c r="C35">
-        <v>349</v>
+        <v>483</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
@@ -3605,7 +3605,7 @@
         <v>21</v>
       </c>
       <c r="C36">
-        <v>350</v>
+        <v>459</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
@@ -3613,7 +3613,7 @@
         <v>22</v>
       </c>
       <c r="C37">
-        <v>333</v>
+        <v>420</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
@@ -3621,13 +3621,13 @@
         <v>23</v>
       </c>
       <c r="C38">
-        <v>274</v>
+        <v>380</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E39">
         <f>SUM(C15, C16, C17, C18, C19, C20, C21, C22, C23, C24, C25, C26, C27, C28, C29, C30, C31, C32, C33, C34, C35, C36, C37, C38)</f>
-        <v>7997</v>
+        <v>10805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>